<commit_message>
updated mac version to 0.0.0.0.6
</commit_message>
<xml_diff>
--- a/examples/shared-gen1.xlsx
+++ b/examples/shared-gen1.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jww/Developer/python/terraformer/gen1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ED165D0-2698-1E41-8D01-6CA492544928}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{057D5DCA-2805-644E-9201-08DDB069522F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3680" yWindow="460" windowWidth="25600" windowHeight="14680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="resourcegroups" sheetId="50" r:id="rId1"/>
-    <sheet name="sshkeys" sheetId="36" r:id="rId2"/>
-    <sheet name="menus" sheetId="49" r:id="rId3"/>
+    <sheet name="acls" sheetId="51" r:id="rId1"/>
+    <sheet name="resourcegroups" sheetId="50" r:id="rId2"/>
+    <sheet name="sshkeys" sheetId="36" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
   <si>
     <t>*name</t>
   </si>
@@ -38,24 +38,6 @@
     <t>~/.ssh/id_rsa.pub</t>
   </si>
   <si>
-    <t>Regions</t>
-  </si>
-  <si>
-    <t>Dallas</t>
-  </si>
-  <si>
-    <t>Frankfurt</t>
-  </si>
-  <si>
-    <t>London</t>
-  </si>
-  <si>
-    <t>Sydney</t>
-  </si>
-  <si>
-    <t>Tokyo</t>
-  </si>
-  <si>
     <t>key1</t>
   </si>
   <si>
@@ -63,6 +45,54 @@
   </si>
   <si>
     <t>rg1</t>
+  </si>
+  <si>
+    <t>*action</t>
+  </si>
+  <si>
+    <t>*source</t>
+  </si>
+  <si>
+    <t>*destination</t>
+  </si>
+  <si>
+    <t>*direction</t>
+  </si>
+  <si>
+    <t>protocol</t>
+  </si>
+  <si>
+    <t>acl_name</t>
+  </si>
+  <si>
+    <t>iacl1rule100</t>
+  </si>
+  <si>
+    <t>allow</t>
+  </si>
+  <si>
+    <t>0.0.0.0/0</t>
+  </si>
+  <si>
+    <t>inbound</t>
+  </si>
+  <si>
+    <t>tcp:80:80</t>
+  </si>
+  <si>
+    <t>acl1</t>
+  </si>
+  <si>
+    <t>iacl1rule200</t>
+  </si>
+  <si>
+    <t>udp:805:807</t>
+  </si>
+  <si>
+    <t>eacl1rule100</t>
+  </si>
+  <si>
+    <t>outbound</t>
   </si>
 </sst>
 </file>
@@ -92,7 +122,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -100,11 +130,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.79998168889431442"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -113,11 +152,44 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="17">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -176,34 +248,49 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{36B7C4F4-4417-5447-AA72-1BF91F584093}" name="Table32" displayName="Table32" ref="A1:B2" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="A1:B2" xr:uid="{DC08D300-10E5-4A45-A724-480E99186CDC}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{5BBC829C-2DF4-684D-9B60-D48E25F59407}" name="*name" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{203C4B8E-FB7F-3A44-8057-2DFE9B641A3D}" name="tags" dataDxfId="5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{21E48744-A952-7940-AA28-62EC0112E485}" name="Table1" displayName="Table1" ref="A1:F4" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="A1:F4" xr:uid="{00881A37-2AAB-7345-9099-83242FC8EDEA}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{4F28E2E0-4CFF-4143-B367-5C91F4FC3202}" name="*name" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{CF63E2BE-DE34-4E46-9AFD-390223B4637F}" name="*action" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{2E2E2F36-8F78-D14E-8D0D-50B4D2447E76}" name="*source" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{E97143B3-EFDF-E04E-8C0E-A94AA99CD532}" name="*destination" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{48D46AFA-BC91-784A-BE49-A490470034B0}" name="*direction" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{FF415E2F-606D-EF45-860F-7D1B404CCEF0}" name="protocol" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D18409AA-A6BC-C848-A5DF-F5A05474C1AC}" name="Table3" displayName="Table3" ref="A1:B2" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="A1:B2" xr:uid="{DC08D300-10E5-4A45-A724-480E99186CDC}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{3D71B74E-F0FC-E741-B93E-48B8E368098C}" name="*name" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{DBF7863C-BAD4-C843-903F-D04426BFF587}" name="*public_key" dataDxfId="1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C9C3A828-49D1-2E43-B224-97644A141F78}" name="Table2" displayName="Table2" ref="H1:H2" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="H1:H2" xr:uid="{1E645224-6427-3946-AE0C-8455A88C5D34}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{2F090AC0-C5D2-A346-B27C-46930D36C0D8}" name="acl_name"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{18DBD3B2-0D47-9A4F-A462-3D3C1EA67CB0}" name="Table47" displayName="Table47" ref="A1:A6" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:A6" xr:uid="{4B461739-B056-7441-ADE3-1EBA104D9E4E}"/>
-  <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{2F84416C-3C6A-5F4E-96FD-E2DB92D4CDB8}" name="Regions"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{36B7C4F4-4417-5447-AA72-1BF91F584093}" name="Table32" displayName="Table32" ref="A1:B2" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+  <autoFilter ref="A1:B2" xr:uid="{DC08D300-10E5-4A45-A724-480E99186CDC}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{5BBC829C-2DF4-684D-9B60-D48E25F59407}" name="*name" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{203C4B8E-FB7F-3A44-8057-2DFE9B641A3D}" name="tags" dataDxfId="13"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D18409AA-A6BC-C848-A5DF-F5A05474C1AC}" name="Table3" displayName="Table3" ref="A1:B2" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A1:B2" xr:uid="{DC08D300-10E5-4A45-A724-480E99186CDC}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{3D71B74E-F0FC-E741-B93E-48B8E368098C}" name="*name" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{DBF7863C-BAD4-C843-903F-D04426BFF587}" name="*public_key" dataDxfId="9"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -469,10 +556,116 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BB1E312-169D-1347-B6FE-BF4C770C3337}">
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="7" max="7" width="1.83203125" customWidth="1"/>
+    <col min="8" max="8" width="15.83203125" customWidth="1"/>
+    <col min="9" max="9" width="18.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="2">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75153148-6D2F-7646-AF92-40BBFB0DCDC0}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -484,12 +677,12 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1"/>
     </row>
@@ -501,7 +694,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34D3E930-7386-4478-9099-4EC8B39AF425}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -522,60 +715,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83121959-1082-4F4D-87C7-A880D5B9F0C5}">
-  <dimension ref="A1:A6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="1.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>